<commit_message>
Some more styling and HTML
</commit_message>
<xml_diff>
--- a/public-files/decks/Card Info.xlsx
+++ b/public-files/decks/Card Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Family Data\JRB\Projects\Splendor\public-files\decks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15933D2B-18DD-4896-9599-BC9F9EDD6FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D4DDFB-F490-4C17-BD86-7490D093DB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5877EE35-45CC-4D57-B78D-29EC13D3D150}"/>
+    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5877EE35-45CC-4D57-B78D-29EC13D3D150}"/>
   </bookViews>
   <sheets>
     <sheet name="Blue" sheetId="1" r:id="rId1"/>
@@ -857,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D9CD0B-9563-401B-9080-9443D8C4F3B9}">
-  <dimension ref="A2:M24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,9 +876,31 @@
     <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="51" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G1">
+        <f>SUM(G3:G22)</f>
+        <v>43</v>
+      </c>
+      <c r="H1">
+        <f t="shared" ref="H1:K1" si="0">SUM(H3:H22)</f>
+        <v>43</v>
+      </c>
+      <c r="I1">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="J1">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="K1">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -944,13 +966,13 @@
         <v>0</v>
       </c>
       <c r="M3" t="str">
-        <f>_xlfn.CONCAT("const ",C3," = new BlueCard(",D3,$A$3,E3,$A$3,F3,$A$3,G3,$A$3,H3,$A$3,I3,$A$3,J3,$A$3,K3,")")</f>
-        <v>const BC01 = new BlueCard("01", 5, "black", 3, 7, 0, 0, 0)</v>
+        <f>_xlfn.CONCAT("const ",C3," = new Card(",D3,$A$3,E3,$A$3,F3,$A$3,G3,$A$3,H3,$A$3,I3,$A$3,J3,$A$3,K3,")")</f>
+        <v>const BC01 = new Card("01", 5, "black", 3, 7, 0, 0, 0)</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B21" si="0">C4&amp;", "</f>
+        <f t="shared" ref="B4:B21" si="1">C4&amp;", "</f>
         <v xml:space="preserve">BC02, </v>
       </c>
       <c r="C4" t="s">
@@ -981,13 +1003,13 @@
         <v>0</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" ref="M4:M22" si="1">_xlfn.CONCAT("const ",C4," = new BlueCard(",D4,$A$3,E4,$A$3,F4,$A$3,G4,$A$3,H4,$A$3,I4,$A$3,J4,$A$3,K4,")")</f>
-        <v>const BC02 = new BlueCard("02", 4, "black", 3, 6, 3, 0, 0)</v>
+        <f t="shared" ref="M4:M22" si="2">_xlfn.CONCAT("const ",C4," = new Card(",D4,$A$3,E4,$A$3,F4,$A$3,G4,$A$3,H4,$A$3,I4,$A$3,J4,$A$3,K4,")")</f>
+        <v>const BC02 = new Card("02", 4, "black", 3, 6, 3, 0, 0)</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC03, </v>
       </c>
       <c r="C5" t="s">
@@ -1018,13 +1040,13 @@
         <v>0</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC03 = new BlueCard("03", 4, "black", 0, 7, 0, 0, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const BC03 = new Card("03", 4, "black", 0, 7, 0, 0, 0)</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC04, </v>
       </c>
       <c r="C6" t="s">
@@ -1055,13 +1077,13 @@
         <v>3</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC04 = new BlueCard("04", 3, "black", 0, 3, 5, 3, 3)</v>
+        <f t="shared" si="2"/>
+        <v>const BC04 = new Card("04", 3, "black", 0, 3, 5, 3, 3)</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC05, </v>
       </c>
       <c r="C7" t="s">
@@ -1092,13 +1114,13 @@
         <v>0</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC05 = new BlueCard("05", 5, "red", 0, 3, 7, 0, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const BC05 = new Card("05", 5, "red", 0, 3, 7, 0, 0)</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC06, </v>
       </c>
       <c r="C8" t="s">
@@ -1129,13 +1151,13 @@
         <v>0</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC06 = new BlueCard("06", 4, "red", 0, 3, 6, 3, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const BC06 = new Card("06", 4, "red", 0, 3, 6, 3, 0)</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC07, </v>
       </c>
       <c r="C9" t="s">
@@ -1166,13 +1188,13 @@
         <v>0</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC07 = new BlueCard("07", 4, "red", 0, 0, 7, 0, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const BC07 = new Card("07", 4, "red", 0, 0, 7, 0, 0)</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC08, </v>
       </c>
       <c r="C10" t="s">
@@ -1203,13 +1225,13 @@
         <v>3</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC08 = new BlueCard("08", 3, "red", 3, 0, 3, 5, 3)</v>
+        <f t="shared" si="2"/>
+        <v>const BC08 = new Card("08", 3, "red", 3, 0, 3, 5, 3)</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC09, </v>
       </c>
       <c r="C11" t="s">
@@ -1240,13 +1262,13 @@
         <v>0</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC09 = new BlueCard("09", 5, "green", 0, 0, 3, 7, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const BC09 = new Card("09", 5, "green", 0, 0, 3, 7, 0)</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC10, </v>
       </c>
       <c r="C12" t="s">
@@ -1277,13 +1299,13 @@
         <v>3</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC10 = new BlueCard("10", 4, "green", 0, 0, 3, 6, 3)</v>
+        <f t="shared" si="2"/>
+        <v>const BC10 = new Card("10", 4, "green", 0, 0, 3, 6, 3)</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC11, </v>
       </c>
       <c r="C13" t="s">
@@ -1314,13 +1336,13 @@
         <v>0</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC11 = new BlueCard("11", 4, "green", 0, 0, 0, 7, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const BC11 = new Card("11", 4, "green", 0, 0, 0, 7, 0)</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC12, </v>
       </c>
       <c r="C14" t="s">
@@ -1351,13 +1373,13 @@
         <v>5</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC12 = new BlueCard("12", 3, "green", 3, 3, 0, 3, 5)</v>
+        <f t="shared" si="2"/>
+        <v>const BC12 = new Card("12", 3, "green", 3, 3, 0, 3, 5)</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC13, </v>
       </c>
       <c r="C15" t="s">
@@ -1388,13 +1410,13 @@
         <v>7</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC13 = new BlueCard("13", 5, "blue", 0, 0, 0, 3, 7)</v>
+        <f t="shared" si="2"/>
+        <v>const BC13 = new Card("13", 5, "blue", 0, 0, 0, 3, 7)</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC14, </v>
       </c>
       <c r="C16" t="s">
@@ -1425,13 +1447,13 @@
         <v>6</v>
       </c>
       <c r="M16" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC14 = new BlueCard("14", 4, "blue", 3, 0, 0, 3, 6)</v>
+        <f t="shared" si="2"/>
+        <v>const BC14 = new Card("14", 4, "blue", 3, 0, 0, 3, 6)</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC15, </v>
       </c>
       <c r="C17" t="s">
@@ -1462,13 +1484,13 @@
         <v>7</v>
       </c>
       <c r="M17" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC15 = new BlueCard("15", 4, "blue", 0, 0, 0, 0, 7)</v>
+        <f t="shared" si="2"/>
+        <v>const BC15 = new Card("15", 4, "blue", 0, 0, 0, 0, 7)</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC16, </v>
       </c>
       <c r="C18" t="s">
@@ -1499,13 +1521,13 @@
         <v>3</v>
       </c>
       <c r="M18" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC16 = new BlueCard("16", 3, "blue", 5, 3, 3, 0, 3)</v>
+        <f t="shared" si="2"/>
+        <v>const BC16 = new Card("16", 3, "blue", 5, 3, 3, 0, 3)</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC17, </v>
       </c>
       <c r="C19" t="s">
@@ -1536,13 +1558,13 @@
         <v>3</v>
       </c>
       <c r="M19" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC17 = new BlueCard("17", 5, "white", 7, 0, 0, 0, 3)</v>
+        <f t="shared" si="2"/>
+        <v>const BC17 = new Card("17", 5, "white", 7, 0, 0, 0, 3)</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC18, </v>
       </c>
       <c r="C20" t="s">
@@ -1573,13 +1595,13 @@
         <v>3</v>
       </c>
       <c r="M20" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC18 = new BlueCard("18", 4, "white", 6, 3, 0, 0, 3)</v>
+        <f t="shared" si="2"/>
+        <v>const BC18 = new Card("18", 4, "white", 6, 3, 0, 0, 3)</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">BC19, </v>
       </c>
       <c r="C21" t="s">
@@ -1610,8 +1632,8 @@
         <v>0</v>
       </c>
       <c r="M21" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC19 = new BlueCard("19", 4, "white", 7, 0, 0, 0, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const BC19 = new Card("19", 4, "white", 7, 0, 0, 0, 0)</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
@@ -1647,14 +1669,14 @@
         <v>0</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" si="1"/>
-        <v>const BC20 = new BlueCard("20", 3, "white", 3, 5, 3, 3, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const BC20 = new Card("20", 3, "white", 3, 5, 3, 3, 0)</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
-        <f>_xlfn.CONCAT("return [",B3:B22,"]")</f>
-        <v>return [BC01, BC02, BC03, BC04, BC05, BC06, BC07, BC08, BC09, BC10, BC11, BC12, BC13, BC14, BC15, BC16, BC17, BC18, BC19, BC20]</v>
+        <f>_xlfn.CONCAT("activeDeck.splice(0, oldCards, ",B3:B22,")")</f>
+        <v>activeDeck.splice(0, oldCards, BC01, BC02, BC03, BC04, BC05, BC06, BC07, BC08, BC09, BC10, BC11, BC12, BC13, BC14, BC15, BC16, BC17, BC18, BC19, BC20)</v>
       </c>
     </row>
   </sheetData>
@@ -1666,10 +1688,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{022C243F-DF28-48EF-AEDB-F98EB71F7DC3}">
-  <dimension ref="A2:M34"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1685,9 +1707,31 @@
     <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G1">
+        <f>SUM(G3:G32)</f>
+        <v>41</v>
+      </c>
+      <c r="H1">
+        <f t="shared" ref="H1:K1" si="0">SUM(H3:H32)</f>
+        <v>41</v>
+      </c>
+      <c r="I1">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="J1">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="K1">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -1753,13 +1797,13 @@
         <v>0</v>
       </c>
       <c r="M3" t="str">
-        <f>_xlfn.CONCAT("const ",C3," = new YellowCard(",D3,$A$3,E3,$A$3,F3,$A$3,G3,$A$3,H3,$A$3,I3,$A$3,J3,$A$3,K3,")")</f>
-        <v>const YC01 = new YellowCard("01", 3, "black", 6, 0, 0, 0, 0)</v>
+        <f>_xlfn.CONCAT("const ",C3," = new Card(",D3,$A$3,E3,$A$3,F3,$A$3,G3,$A$3,H3,$A$3,I3,$A$3,J3,$A$3,K3,")")</f>
+        <v>const YC01 = new Card("01", 3, "black", 6, 0, 0, 0, 0)</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B31" si="0">C4&amp;", "</f>
+        <f t="shared" ref="B4:B31" si="1">C4&amp;", "</f>
         <v xml:space="preserve">YC02, </v>
       </c>
       <c r="C4" t="s">
@@ -1790,13 +1834,13 @@
         <v>5</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" ref="M4:M32" si="1">_xlfn.CONCAT("const ",C4," = new YellowCard(",D4,$A$3,E4,$A$3,F4,$A$3,G4,$A$3,H4,$A$3,I4,$A$3,J4,$A$3,K4,")")</f>
-        <v>const YC02 = new YellowCard("02", 2, "black", 0, 0, 0, 0, 5)</v>
+        <f t="shared" ref="M4:M32" si="2">_xlfn.CONCAT("const ",C4," = new Card(",D4,$A$3,E4,$A$3,F4,$A$3,G4,$A$3,H4,$A$3,I4,$A$3,J4,$A$3,K4,")")</f>
+        <v>const YC02 = new Card("02", 2, "black", 0, 0, 0, 0, 5)</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC03, </v>
       </c>
       <c r="C5" t="s">
@@ -1827,13 +1871,13 @@
         <v>0</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC03 = new YellowCard("03", 2, "black", 0, 2, 4, 1, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC03 = new Card("03", 2, "black", 0, 2, 4, 1, 0)</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC04, </v>
       </c>
       <c r="C6" t="s">
@@ -1864,13 +1908,13 @@
         <v>0</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC04 = new YellowCard("04", 2, "black", 0, 3, 5, 0, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC04 = new Card("04", 2, "black", 0, 3, 5, 0, 0)</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC05, </v>
       </c>
       <c r="C7" t="s">
@@ -1901,13 +1945,13 @@
         <v>3</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC05 = new YellowCard("05", 1, "black", 0, 0, 2, 2, 3)</v>
+        <f t="shared" si="2"/>
+        <v>const YC05 = new Card("05", 1, "black", 0, 0, 2, 2, 3)</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC06, </v>
       </c>
       <c r="C8" t="s">
@@ -1938,13 +1982,13 @@
         <v>3</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC06 = new YellowCard("06", 1, "black", 2, 0, 3, 0, 3)</v>
+        <f t="shared" si="2"/>
+        <v>const YC06 = new Card("06", 1, "black", 2, 0, 3, 0, 3)</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC07, </v>
       </c>
       <c r="C9" t="s">
@@ -1975,13 +2019,13 @@
         <v>0</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC07 = new YellowCard("07", 3, "red", 0, 6, 0, 0, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC07 = new Card("07", 3, "red", 0, 6, 0, 0, 0)</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC08, </v>
       </c>
       <c r="C10" t="s">
@@ -2012,13 +2056,13 @@
         <v>0</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC08 = new YellowCard("08", 2, "red", 5, 0, 0, 0, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC08 = new Card("08", 2, "red", 5, 0, 0, 0, 0)</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC09, </v>
       </c>
       <c r="C11" t="s">
@@ -2049,13 +2093,13 @@
         <v>1</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC09 = new YellowCard("09", 2, "red", 0, 0, 2, 4, 1)</v>
+        <f t="shared" si="2"/>
+        <v>const YC09 = new Card("09", 2, "red", 0, 0, 2, 4, 1)</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC10, </v>
       </c>
       <c r="C12" t="s">
@@ -2086,13 +2130,13 @@
         <v>3</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC10 = new YellowCard("10", 2, "red", 5, 0, 0, 0, 3)</v>
+        <f t="shared" si="2"/>
+        <v>const YC10 = new Card("10", 2, "red", 5, 0, 0, 0, 3)</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC11, </v>
       </c>
       <c r="C13" t="s">
@@ -2123,13 +2167,13 @@
         <v>2</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC11 = new YellowCard("11", 1, "red", 3, 2, 0, 0, 2)</v>
+        <f t="shared" si="2"/>
+        <v>const YC11 = new Card("11", 1, "red", 3, 2, 0, 0, 2)</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC12, </v>
       </c>
       <c r="C14" t="s">
@@ -2160,13 +2204,13 @@
         <v>0</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC12 = new YellowCard("12", 1, "red", 3, 2, 0, 3, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC12 = new Card("12", 1, "red", 3, 2, 0, 3, 0)</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC13, </v>
       </c>
       <c r="C15" t="s">
@@ -2197,13 +2241,13 @@
         <v>0</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC13 = new YellowCard("13", 3, "green", 0, 0, 6, 0, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC13 = new Card("13", 3, "green", 0, 0, 6, 0, 0)</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC14, </v>
       </c>
       <c r="C16" t="s">
@@ -2234,13 +2278,13 @@
         <v>0</v>
       </c>
       <c r="M16" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC14 = new YellowCard("14", 2, "green", 0, 0, 5, 0, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC14 = new Card("14", 2, "green", 0, 0, 5, 0, 0)</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC15, </v>
       </c>
       <c r="C17" t="s">
@@ -2271,13 +2315,13 @@
         <v>4</v>
       </c>
       <c r="M17" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC15 = new YellowCard("15", 2, "green", 1, 0, 0, 2, 4)</v>
+        <f t="shared" si="2"/>
+        <v>const YC15 = new Card("15", 2, "green", 1, 0, 0, 2, 4)</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC16, </v>
       </c>
       <c r="C18" t="s">
@@ -2308,13 +2352,13 @@
         <v>0</v>
       </c>
       <c r="M18" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC16 = new YellowCard("16", 2, "green", 0, 0, 3, 5, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC16 = new Card("16", 2, "green", 0, 0, 3, 5, 0)</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC17, </v>
       </c>
       <c r="C19" t="s">
@@ -2345,13 +2389,13 @@
         <v>2</v>
       </c>
       <c r="M19" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC17 = new YellowCard("17", 1, "green", 2, 0, 0, 3, 2)</v>
+        <f t="shared" si="2"/>
+        <v>const YC17 = new Card("17", 1, "green", 2, 0, 0, 3, 2)</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC18, </v>
       </c>
       <c r="C20" t="s">
@@ -2382,13 +2426,13 @@
         <v>3</v>
       </c>
       <c r="M20" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC18 = new YellowCard("18", 1, "green", 0, 3, 2, 0, 3)</v>
+        <f t="shared" si="2"/>
+        <v>const YC18 = new Card("18", 1, "green", 0, 3, 2, 0, 3)</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC19, </v>
       </c>
       <c r="C21" t="s">
@@ -2419,13 +2463,13 @@
         <v>0</v>
       </c>
       <c r="M21" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC19 = new YellowCard("19", 3, "blue", 0, 0, 0, 6, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC19 = new Card("19", 3, "blue", 0, 0, 0, 6, 0)</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC20, </v>
       </c>
       <c r="C22" t="s">
@@ -2456,13 +2500,13 @@
         <v>0</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC20 = new YellowCard("20", 2, "blue", 0, 0, 0, 5, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC20 = new Card("20", 2, "blue", 0, 0, 0, 5, 0)</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC21, </v>
       </c>
       <c r="C23" t="s">
@@ -2493,13 +2537,13 @@
         <v>2</v>
       </c>
       <c r="M23" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC21 = new YellowCard("21", 2, "blue", 4, 1, 0, 0, 2)</v>
+        <f t="shared" si="2"/>
+        <v>const YC21 = new Card("21", 2, "blue", 4, 1, 0, 0, 2)</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC22, </v>
       </c>
       <c r="C24" t="s">
@@ -2530,13 +2574,13 @@
         <v>5</v>
       </c>
       <c r="M24" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC22 = new YellowCard("22", 2, "blue", 0, 0, 0, 3, 5)</v>
+        <f t="shared" si="2"/>
+        <v>const YC22 = new Card("22", 2, "blue", 0, 0, 0, 3, 5)</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC23, </v>
       </c>
       <c r="C25" t="s">
@@ -2567,13 +2611,13 @@
         <v>0</v>
       </c>
       <c r="M25" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC23 = new YellowCard("23", 1, "blue", 0, 3, 2, 2, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC23 = new Card("23", 1, "blue", 0, 3, 2, 2, 0)</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC24, </v>
       </c>
       <c r="C26" t="s">
@@ -2604,13 +2648,13 @@
         <v>0</v>
       </c>
       <c r="M26" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC24 = new YellowCard("24", 1, "blue", 3, 0, 3, 2, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC24 = new Card("24", 1, "blue", 3, 0, 3, 2, 0)</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC25, </v>
       </c>
       <c r="C27" t="s">
@@ -2641,13 +2685,13 @@
         <v>6</v>
       </c>
       <c r="M27" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC25 = new YellowCard("25", 3, "white", 0, 0, 0, 0, 6)</v>
+        <f t="shared" si="2"/>
+        <v>const YC25 = new Card("25", 3, "white", 0, 0, 0, 0, 6)</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC26, </v>
       </c>
       <c r="C28" t="s">
@@ -2678,13 +2722,13 @@
         <v>0</v>
       </c>
       <c r="M28" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC26 = new YellowCard("26", 2, "white", 0, 5, 0, 0, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC26 = new Card("26", 2, "white", 0, 5, 0, 0, 0)</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC27, </v>
       </c>
       <c r="C29" t="s">
@@ -2715,13 +2759,13 @@
         <v>0</v>
       </c>
       <c r="M29" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC27 = new YellowCard("27", 2, "white", 2, 4, 1, 0, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC27 = new Card("27", 2, "white", 2, 4, 1, 0, 0)</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC28, </v>
       </c>
       <c r="C30" t="s">
@@ -2752,13 +2796,13 @@
         <v>0</v>
       </c>
       <c r="M30" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC28 = new YellowCard("28", 2, "white", 3, 5, 0, 0, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC28 = new Card("28", 2, "white", 3, 5, 0, 0, 0)</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">YC29, </v>
       </c>
       <c r="C31" t="s">
@@ -2789,8 +2833,8 @@
         <v>0</v>
       </c>
       <c r="M31" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC29 = new YellowCard("29", 1, "white", 2, 2, 3, 0, 0)</v>
+        <f t="shared" si="2"/>
+        <v>const YC29 = new Card("29", 1, "white", 2, 2, 3, 0, 0)</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
@@ -2826,14 +2870,14 @@
         <v>2</v>
       </c>
       <c r="M32" t="str">
-        <f t="shared" si="1"/>
-        <v>const YC30 = new YellowCard("30", 1, "white", 0, 3, 0, 3, 2)</v>
+        <f t="shared" si="2"/>
+        <v>const YC30 = new Card("30", 1, "white", 0, 3, 0, 3, 2)</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
-        <f>_xlfn.CONCAT("return [",B3:B32,"]")</f>
-        <v>return [YC01, YC02, YC03, YC04, YC05, YC06, YC07, YC08, YC09, YC10, YC11, YC12, YC13, YC14, YC15, YC16, YC17, YC18, YC19, YC20, YC21, YC22, YC23, YC24, YC25, YC26, YC27, YC28, YC29, YC30]</v>
+        <f>_xlfn.CONCAT("activeDeck.splice(0, oldCards, ",B3:B32,")")</f>
+        <v>activeDeck.splice(0, oldCards, YC01, YC02, YC03, YC04, YC05, YC06, YC07, YC08, YC09, YC10, YC11, YC12, YC13, YC14, YC15, YC16, YC17, YC18, YC19, YC20, YC21, YC22, YC23, YC24, YC25, YC26, YC27, YC28, YC29, YC30)</v>
       </c>
     </row>
   </sheetData>
@@ -2845,10 +2889,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8FDFBD-F5B4-463C-9495-E14CEFB5E2DB}">
-  <dimension ref="A2:M44"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2864,9 +2908,31 @@
     <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G1">
+        <f>SUM(G3:G42)</f>
+        <v>33</v>
+      </c>
+      <c r="H1">
+        <f t="shared" ref="H1:K1" si="0">SUM(H3:H42)</f>
+        <v>33</v>
+      </c>
+      <c r="I1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="J1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="K1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -2931,18 +2997,14 @@
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3">
-        <f>SUM(G3:K3)</f>
-        <v>4</v>
-      </c>
       <c r="M3" t="str">
-        <f>_xlfn.CONCAT("const ",C3," = new GreenCard(",D3,$A$3,E3,$A$3,F3,$A$3,G3,$A$3,H3,$A$3,I3,$A$3,J3,$A$3,K3,")")</f>
-        <v>const GC01 = new GreenCard("01", 1, "black", 0, 0, 0, 4, 0)</v>
+        <f>_xlfn.CONCAT("const ",C3," = new Card(",D3,$A$3,E3,$A$3,F3,$A$3,G3,$A$3,H3,$A$3,I3,$A$3,J3,$A$3,K3,")")</f>
+        <v>const GC01 = new Card("01", 1, "black", 0, 0, 0, 4, 0)</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B41" si="0">C4&amp;", "</f>
+        <f t="shared" ref="B4:B41" si="1">C4&amp;", "</f>
         <v xml:space="preserve">GC02, </v>
       </c>
       <c r="C4" t="s">
@@ -2972,18 +3034,14 @@
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4">
-        <f t="shared" ref="L4:L42" si="1">SUM(G4:K4)</f>
-        <v>3</v>
-      </c>
       <c r="M4" t="str">
-        <f t="shared" ref="M4:M42" si="2">_xlfn.CONCAT("const ",C4," = new GreenCard(",D4,$A$3,E4,$A$3,F4,$A$3,G4,$A$3,H4,$A$3,I4,$A$3,J4,$A$3,K4,")")</f>
-        <v>const GC02 = new GreenCard("02", 0, "black", 0, 1, 2, 0, 0)</v>
+        <f t="shared" ref="M4:M42" si="2">_xlfn.CONCAT("const ",C4," = new Card(",D4,$A$3,E4,$A$3,F4,$A$3,G4,$A$3,H4,$A$3,I4,$A$3,J4,$A$3,K4,")")</f>
+        <v>const GC02 = new Card("02", 0, "black", 0, 1, 2, 0, 0)</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC03, </v>
       </c>
       <c r="C5" t="s">
@@ -3013,18 +3071,14 @@
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
       <c r="M5" t="str">
         <f t="shared" si="2"/>
-        <v>const GC03 = new GreenCard("03", 0, "black", 0, 0, 3, 0, 0)</v>
+        <v>const GC03 = new Card("03", 0, "black", 0, 0, 3, 0, 0)</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC04, </v>
       </c>
       <c r="C6" t="s">
@@ -3054,18 +3108,14 @@
       <c r="K6">
         <v>1</v>
       </c>
-      <c r="L6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
       <c r="M6" t="str">
         <f t="shared" si="2"/>
-        <v>const GC04 = new GreenCard("04", 0, "black", 0, 1, 1, 1, 1)</v>
+        <v>const GC04 = new Card("04", 0, "black", 0, 1, 1, 1, 1)</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC05, </v>
       </c>
       <c r="C7" t="s">
@@ -3095,18 +3145,14 @@
       <c r="K7">
         <v>2</v>
       </c>
-      <c r="L7">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
       <c r="M7" t="str">
         <f t="shared" si="2"/>
-        <v>const GC05 = new GreenCard("05", 0, "black", 0, 0, 2, 0, 2)</v>
+        <v>const GC05 = new Card("05", 0, "black", 0, 0, 2, 0, 2)</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC06, </v>
       </c>
       <c r="C8" t="s">
@@ -3136,18 +3182,14 @@
       <c r="K8">
         <v>1</v>
       </c>
-      <c r="L8">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="M8" t="str">
         <f t="shared" si="2"/>
-        <v>const GC06 = new GreenCard("06", 0, "black", 0, 1, 1, 2, 1)</v>
+        <v>const GC06 = new Card("06", 0, "black", 0, 1, 1, 2, 1)</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC07, </v>
       </c>
       <c r="C9" t="s">
@@ -3177,18 +3219,14 @@
       <c r="K9">
         <v>2</v>
       </c>
-      <c r="L9">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="M9" t="str">
         <f t="shared" si="2"/>
-        <v>const GC07 = new GreenCard("07", 0, "black", 0, 1, 0, 2, 2)</v>
+        <v>const GC07 = new Card("07", 0, "black", 0, 1, 0, 2, 2)</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC08, </v>
       </c>
       <c r="C10" t="s">
@@ -3218,18 +3256,14 @@
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="M10" t="str">
         <f t="shared" si="2"/>
-        <v>const GC08 = new GreenCard("08", 0, "black", 1, 3, 1, 0, 0)</v>
+        <v>const GC08 = new Card("08", 0, "black", 1, 3, 1, 0, 0)</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC09, </v>
       </c>
       <c r="C11" t="s">
@@ -3259,18 +3293,14 @@
       <c r="K11">
         <v>4</v>
       </c>
-      <c r="L11">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
       <c r="M11" t="str">
         <f t="shared" si="2"/>
-        <v>const GC09 = new GreenCard("09", 1, "red", 0, 0, 0, 0, 4)</v>
+        <v>const GC09 = new Card("09", 1, "red", 0, 0, 0, 0, 4)</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC10, </v>
       </c>
       <c r="C12" t="s">
@@ -3300,18 +3330,14 @@
       <c r="K12">
         <v>0</v>
       </c>
-      <c r="L12">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
       <c r="M12" t="str">
         <f t="shared" si="2"/>
-        <v>const GC10 = new GreenCard("10", 0, "red", 0, 0, 1, 2, 0)</v>
+        <v>const GC10 = new Card("10", 0, "red", 0, 0, 1, 2, 0)</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC11, </v>
       </c>
       <c r="C13" t="s">
@@ -3341,18 +3367,14 @@
       <c r="K13">
         <v>3</v>
       </c>
-      <c r="L13">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
       <c r="M13" t="str">
         <f t="shared" si="2"/>
-        <v>const GC11 = new GreenCard("11", 0, "red", 0, 0, 0, 0, 3)</v>
+        <v>const GC11 = new Card("11", 0, "red", 0, 0, 0, 0, 3)</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC12, </v>
       </c>
       <c r="C14" t="s">
@@ -3382,18 +3404,14 @@
       <c r="K14">
         <v>1</v>
       </c>
-      <c r="L14">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
       <c r="M14" t="str">
         <f t="shared" si="2"/>
-        <v>const GC12 = new GreenCard("12", 0, "red", 1, 0, 1, 1, 1)</v>
+        <v>const GC12 = new Card("12", 0, "red", 1, 0, 1, 1, 1)</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC13, </v>
       </c>
       <c r="C15" t="s">
@@ -3423,18 +3441,14 @@
       <c r="K15">
         <v>2</v>
       </c>
-      <c r="L15">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
       <c r="M15" t="str">
         <f t="shared" si="2"/>
-        <v>const GC13 = new GreenCard("13", 0, "red", 0, 2, 0, 0, 2)</v>
+        <v>const GC13 = new Card("13", 0, "red", 0, 2, 0, 0, 2)</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC14, </v>
       </c>
       <c r="C16" t="s">
@@ -3464,18 +3478,14 @@
       <c r="K16">
         <v>2</v>
       </c>
-      <c r="L16">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="M16" t="str">
         <f t="shared" si="2"/>
-        <v>const GC14 = new GreenCard("14", 0, "red", 1, 0, 1, 1, 2)</v>
+        <v>const GC14 = new Card("14", 0, "red", 1, 0, 1, 1, 2)</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC15, </v>
       </c>
       <c r="C17" t="s">
@@ -3505,18 +3515,14 @@
       <c r="K17">
         <v>2</v>
       </c>
-      <c r="L17">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="M17" t="str">
         <f t="shared" si="2"/>
-        <v>const GC15 = new GreenCard("15", 0, "red", 2, 0, 1, 0, 2)</v>
+        <v>const GC15 = new Card("15", 0, "red", 2, 0, 1, 0, 2)</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC16, </v>
       </c>
       <c r="C18" t="s">
@@ -3546,18 +3552,14 @@
       <c r="K18">
         <v>1</v>
       </c>
-      <c r="L18">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="M18" t="str">
         <f t="shared" si="2"/>
-        <v>const GC16 = new GreenCard("16", 0, "red", 3, 1, 0, 0, 1)</v>
+        <v>const GC16 = new Card("16", 0, "red", 3, 1, 0, 0, 1)</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC17, </v>
       </c>
       <c r="C19" t="s">
@@ -3587,18 +3589,14 @@
       <c r="K19">
         <v>0</v>
       </c>
-      <c r="L19">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
       <c r="M19" t="str">
         <f t="shared" si="2"/>
-        <v>const GC17 = new GreenCard("17", 1, "green", 4, 0, 0, 0, 0)</v>
+        <v>const GC17 = new Card("17", 1, "green", 4, 0, 0, 0, 0)</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC18, </v>
       </c>
       <c r="C20" t="s">
@@ -3628,18 +3626,14 @@
       <c r="K20">
         <v>2</v>
       </c>
-      <c r="L20">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
       <c r="M20" t="str">
         <f t="shared" si="2"/>
-        <v>const GC18 = new GreenCard("18", 0, "green", 0, 0, 0, 1, 2)</v>
+        <v>const GC18 = new Card("18", 0, "green", 0, 0, 0, 1, 2)</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC19, </v>
       </c>
       <c r="C21" t="s">
@@ -3669,18 +3663,14 @@
       <c r="K21">
         <v>0</v>
       </c>
-      <c r="L21">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
       <c r="M21" t="str">
         <f t="shared" si="2"/>
-        <v>const GC19 = new GreenCard("19", 0, "green", 0, 3, 0, 0, 0)</v>
+        <v>const GC19 = new Card("19", 0, "green", 0, 3, 0, 0, 0)</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC20, </v>
       </c>
       <c r="C22" t="s">
@@ -3710,18 +3700,14 @@
       <c r="K22">
         <v>1</v>
       </c>
-      <c r="L22">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
       <c r="M22" t="str">
         <f t="shared" si="2"/>
-        <v>const GC20 = new GreenCard("20", 0, "green", 1, 1, 0, 1, 1)</v>
+        <v>const GC20 = new Card("20", 0, "green", 1, 1, 0, 1, 1)</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC21, </v>
       </c>
       <c r="C23" t="s">
@@ -3751,18 +3737,14 @@
       <c r="K23">
         <v>0</v>
       </c>
-      <c r="L23">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
       <c r="M23" t="str">
         <f t="shared" si="2"/>
-        <v>const GC21 = new GreenCard("21", 0, "green", 0, 2, 0, 2, 0)</v>
+        <v>const GC21 = new Card("21", 0, "green", 0, 2, 0, 2, 0)</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC22, </v>
       </c>
       <c r="C24" t="s">
@@ -3792,18 +3774,14 @@
       <c r="K24">
         <v>1</v>
       </c>
-      <c r="L24">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="M24" t="str">
         <f t="shared" si="2"/>
-        <v>const GC22 = new GreenCard("22", 0, "green", 2, 1, 0, 1, 1)</v>
+        <v>const GC22 = new Card("22", 0, "green", 2, 1, 0, 1, 1)</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC23, </v>
       </c>
       <c r="C25" t="s">
@@ -3833,18 +3811,14 @@
       <c r="K25">
         <v>0</v>
       </c>
-      <c r="L25">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="M25" t="str">
         <f t="shared" si="2"/>
-        <v>const GC23 = new GreenCard("23", 0, "green", 2, 2, 0, 1, 0)</v>
+        <v>const GC23 = new Card("23", 0, "green", 2, 2, 0, 1, 0)</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC24, </v>
       </c>
       <c r="C26" t="s">
@@ -3874,18 +3848,14 @@
       <c r="K26">
         <v>1</v>
       </c>
-      <c r="L26">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="M26" t="str">
         <f t="shared" si="2"/>
-        <v>const GC24 = new GreenCard("24", 0, "green", 0, 0, 1, 3, 1)</v>
+        <v>const GC24 = new Card("24", 0, "green", 0, 0, 1, 3, 1)</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC25, </v>
       </c>
       <c r="C27" t="s">
@@ -3915,18 +3885,14 @@
       <c r="K27">
         <v>0</v>
       </c>
-      <c r="L27">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
       <c r="M27" t="str">
         <f t="shared" si="2"/>
-        <v>const GC25 = new GreenCard("25", 1, "blue", 0, 4, 0, 0, 0)</v>
+        <v>const GC25 = new Card("25", 1, "blue", 0, 4, 0, 0, 0)</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC26, </v>
       </c>
       <c r="C28" t="s">
@@ -3956,18 +3922,14 @@
       <c r="K28">
         <v>1</v>
       </c>
-      <c r="L28">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
       <c r="M28" t="str">
         <f t="shared" si="2"/>
-        <v>const GC26 = new GreenCard("26", 0, "blue", 2, 0, 0, 0, 1)</v>
+        <v>const GC26 = new Card("26", 0, "blue", 2, 0, 0, 0, 1)</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC27, </v>
       </c>
       <c r="C29" t="s">
@@ -3997,18 +3959,14 @@
       <c r="K29">
         <v>0</v>
       </c>
-      <c r="L29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
       <c r="M29" t="str">
         <f t="shared" si="2"/>
-        <v>const GC27 = new GreenCard("27", 0, "blue", 3, 0, 0, 0, 0)</v>
+        <v>const GC27 = new Card("27", 0, "blue", 3, 0, 0, 0, 0)</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC28, </v>
       </c>
       <c r="C30" t="s">
@@ -4038,18 +3996,14 @@
       <c r="K30">
         <v>1</v>
       </c>
-      <c r="L30">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
       <c r="M30" t="str">
         <f t="shared" si="2"/>
-        <v>const GC28 = new GreenCard("28", 0, "blue", 1, 1, 1, 0, 1)</v>
+        <v>const GC28 = new Card("28", 0, "blue", 1, 1, 1, 0, 1)</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC29, </v>
       </c>
       <c r="C31" t="s">
@@ -4079,18 +4033,14 @@
       <c r="K31">
         <v>0</v>
       </c>
-      <c r="L31">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
       <c r="M31" t="str">
         <f t="shared" si="2"/>
-        <v>const GC29 = new GreenCard("29", 0, "blue", 2, 0, 2, 0, 0)</v>
+        <v>const GC29 = new Card("29", 0, "blue", 2, 0, 2, 0, 0)</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC30, </v>
       </c>
       <c r="C32" t="s">
@@ -4120,18 +4070,14 @@
       <c r="K32">
         <v>1</v>
       </c>
-      <c r="L32">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="M32" t="str">
         <f t="shared" si="2"/>
-        <v>const GC30 = new GreenCard("30", 0, "blue", 1, 2, 1, 0, 1)</v>
+        <v>const GC30 = new Card("30", 0, "blue", 1, 2, 1, 0, 1)</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC31, </v>
       </c>
       <c r="C33" t="s">
@@ -4161,18 +4107,14 @@
       <c r="K33">
         <v>1</v>
       </c>
-      <c r="L33">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="M33" t="str">
         <f t="shared" si="2"/>
-        <v>const GC31 = new GreenCard("31", 0, "blue", 0, 2, 2, 0, 1)</v>
+        <v>const GC31 = new Card("31", 0, "blue", 0, 2, 2, 0, 1)</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC32, </v>
       </c>
       <c r="C34" t="s">
@@ -4202,18 +4144,14 @@
       <c r="K34">
         <v>0</v>
       </c>
-      <c r="L34">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="M34" t="str">
         <f t="shared" si="2"/>
-        <v>const GC32 = new GreenCard("32", 0, "blue", 0, 1, 3, 1, 0)</v>
+        <v>const GC32 = new Card("32", 0, "blue", 0, 1, 3, 1, 0)</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC33, </v>
       </c>
       <c r="C35" t="s">
@@ -4243,18 +4181,14 @@
       <c r="K35">
         <v>0</v>
       </c>
-      <c r="L35">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
       <c r="M35" t="str">
         <f t="shared" si="2"/>
-        <v>const GC33 = new GreenCard("33", 1, "white", 0, 0, 4, 0, 0)</v>
+        <v>const GC33 = new Card("33", 1, "white", 0, 0, 4, 0, 0)</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC34, </v>
       </c>
       <c r="C36" t="s">
@@ -4284,18 +4218,14 @@
       <c r="K36">
         <v>0</v>
       </c>
-      <c r="L36">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
       <c r="M36" t="str">
         <f t="shared" si="2"/>
-        <v>const GC34 = new GreenCard("34", 0, "white", 1, 2, 0, 0, 0)</v>
+        <v>const GC34 = new Card("34", 0, "white", 1, 2, 0, 0, 0)</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC35, </v>
       </c>
       <c r="C37" t="s">
@@ -4325,18 +4255,14 @@
       <c r="K37">
         <v>0</v>
       </c>
-      <c r="L37">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
       <c r="M37" t="str">
         <f t="shared" si="2"/>
-        <v>const GC35 = new GreenCard("35", 0, "white", 0, 0, 0, 3, 0)</v>
+        <v>const GC35 = new Card("35", 0, "white", 0, 0, 0, 3, 0)</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC36, </v>
       </c>
       <c r="C38" t="s">
@@ -4366,18 +4292,14 @@
       <c r="K38">
         <v>0</v>
       </c>
-      <c r="L38">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
       <c r="M38" t="str">
         <f t="shared" si="2"/>
-        <v>const GC36 = new GreenCard("36", 0, "white", 1, 1, 1, 1, 0)</v>
+        <v>const GC36 = new Card("36", 0, "white", 1, 1, 1, 1, 0)</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC37, </v>
       </c>
       <c r="C39" t="s">
@@ -4407,18 +4329,14 @@
       <c r="K39">
         <v>0</v>
       </c>
-      <c r="L39">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
       <c r="M39" t="str">
         <f t="shared" si="2"/>
-        <v>const GC37 = new GreenCard("37", 0, "white", 2, 0, 0, 2, 0)</v>
+        <v>const GC37 = new Card("37", 0, "white", 2, 0, 0, 2, 0)</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC38, </v>
       </c>
       <c r="C40" t="s">
@@ -4448,18 +4366,14 @@
       <c r="K40">
         <v>0</v>
       </c>
-      <c r="L40">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="M40" t="str">
         <f t="shared" si="2"/>
-        <v>const GC38 = new GreenCard("38", 0, "white", 1, 1, 2, 1, 0)</v>
+        <v>const GC38 = new Card("38", 0, "white", 1, 1, 2, 1, 0)</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">GC39, </v>
       </c>
       <c r="C41" t="s">
@@ -4489,13 +4403,9 @@
       <c r="K41">
         <v>0</v>
       </c>
-      <c r="L41">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="M41" t="str">
         <f t="shared" si="2"/>
-        <v>const GC39 = new GreenCard("39", 0, "white", 1, 0, 2, 2, 0)</v>
+        <v>const GC39 = new Card("39", 0, "white", 1, 0, 2, 2, 0)</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
@@ -4530,19 +4440,15 @@
       <c r="K42">
         <v>3</v>
       </c>
-      <c r="L42">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="M42" t="str">
         <f t="shared" si="2"/>
-        <v>const GC40 = new GreenCard("40", 0, "white", 1, 0, 0, 1, 3)</v>
+        <v>const GC40 = new Card("40", 0, "white", 1, 0, 0, 1, 3)</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
-        <f>_xlfn.CONCAT("return [",B3:B42,"]")</f>
-        <v>return [GC01, GC02, GC03, GC04, GC05, GC06, GC07, GC08, GC09, GC10, GC11, GC12, GC13, GC14, GC15, GC16, GC17, GC18, GC19, GC20, GC21, GC22, GC23, GC24, GC25, GC26, GC27, GC28, GC29, GC30, GC31, GC32, GC33, GC34, GC35, GC36, GC37, GC38, GC39, GC40]</v>
+        <f>_xlfn.CONCAT("activeDeck.splice(0, oldCards, ",B3:B42,")")</f>
+        <v>activeDeck.splice(0, oldCards, GC01, GC02, GC03, GC04, GC05, GC06, GC07, GC08, GC09, GC10, GC11, GC12, GC13, GC14, GC15, GC16, GC17, GC18, GC19, GC20, GC21, GC22, GC23, GC24, GC25, GC26, GC27, GC28, GC29, GC30, GC31, GC32, GC33, GC34, GC35, GC36, GC37, GC38, GC39, GC40)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>